<commit_message>
PROS-5326 - CCRU - Spirits
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/HoReCa Spirits 2018.xlsx
+++ b/Projects/CCRU_SAND/Data/HoReCa Spirits 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="102">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -211,13 +211,10 @@
     <t xml:space="preserve">Эсполон Бланко - 0.7л</t>
   </si>
   <si>
-    <t xml:space="preserve">Espolon Reposado - 0,7L</t>
+    <t xml:space="preserve">Espolon Reposado - 0.7L</t>
   </si>
   <si>
     <t xml:space="preserve">Эсполон Репосадо - 0.7л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Espolon Reposado - 0.7L</t>
   </si>
   <si>
     <t xml:space="preserve">Available Bushmills</t>
@@ -509,27 +506,27 @@
   <dimension ref="A1:AN20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="19" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="28" min="24" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.57085020242915"/>
@@ -1063,7 +1060,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K7" s="4" t="n">
         <v>721059707510</v>
@@ -1126,10 +1123,10 @@
         <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>44</v>
@@ -1146,7 +1143,7 @@
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>47</v>
@@ -1201,10 +1198,10 @@
         <v>41</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>44</v>
@@ -1215,7 +1212,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9" s="4" t="n">
         <v>8004160521308</v>
@@ -1278,10 +1275,10 @@
         <v>41</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>44</v>
@@ -1292,7 +1289,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K10" s="4" t="n">
         <v>8004160227606</v>
@@ -1355,10 +1352,10 @@
         <v>41</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>44</v>
@@ -1369,7 +1366,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K11" s="4" t="n">
         <v>8000020000280</v>
@@ -1432,10 +1429,10 @@
         <v>41</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>44</v>
@@ -1446,7 +1443,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K12" s="4" t="n">
         <v>8000020005285</v>
@@ -1509,10 +1506,10 @@
         <v>41</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>44</v>
@@ -1523,7 +1520,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K13" s="4" t="n">
         <v>8000020000013</v>
@@ -1586,10 +1583,10 @@
         <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>44</v>
@@ -1600,7 +1597,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K14" s="4" t="n">
         <v>8000020000020</v>
@@ -1663,10 +1660,10 @@
         <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>44</v>
@@ -1683,7 +1680,7 @@
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>47</v>
@@ -1696,10 +1693,10 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V15" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="V15" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
@@ -1738,10 +1735,10 @@
         <v>41</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>44</v>
@@ -1752,10 +1749,10 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>45</v>
@@ -1773,10 +1770,10 @@
       <c r="S16" s="3"/>
       <c r="T16" s="7"/>
       <c r="U16" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V16" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="V16" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -1815,10 +1812,10 @@
         <v>41</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>44</v>
@@ -1829,10 +1826,10 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>45</v>
@@ -1850,10 +1847,10 @@
       <c r="S17" s="3"/>
       <c r="T17" s="7"/>
       <c r="U17" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V17" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="V17" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -1892,10 +1889,10 @@
         <v>41</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>44</v>
@@ -1912,7 +1909,7 @@
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>47</v>
@@ -1925,10 +1922,10 @@
       <c r="S18" s="3"/>
       <c r="T18" s="7"/>
       <c r="U18" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V18" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="V18" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
@@ -1967,10 +1964,10 @@
         <v>41</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>44</v>
@@ -1987,7 +1984,7 @@
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>47</v>
@@ -2000,10 +1997,10 @@
       <c r="S19" s="3"/>
       <c r="T19" s="7"/>
       <c r="U19" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V19" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="V19" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
@@ -2042,10 +2039,10 @@
         <v>41</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>44</v>
@@ -2056,10 +2053,10 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>45</v>
@@ -2077,10 +2074,10 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V20" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="V20" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>

</xml_diff>